<commit_message>
almost all dataset without CPR inflation
</commit_message>
<xml_diff>
--- a/Stock_Predictor/symbols_names.xlsx
+++ b/Stock_Predictor/symbols_names.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/test/Desktop/Pyhton_Projects/Stock_Predictor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D63FCAD-D809-FE46-BF3D-602FD54981C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471CBD98-D783-1C4E-AF06-4581E7B9A80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14060"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="symbols_names" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="536">
   <si>
     <t>Symbols</t>
   </si>
@@ -1634,12 +1634,15 @@
   </si>
   <si>
     <t>USA CPI R</t>
+  </si>
+  <si>
+    <t>&lt;- od tego zacząć</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2491,10 +2494,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B280"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D280"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+      <selection activeCell="F248" sqref="F248"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4418,7 +4423,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>455</v>
       </c>
@@ -4426,7 +4431,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>457</v>
       </c>
@@ -4434,7 +4439,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>459</v>
       </c>
@@ -4442,7 +4447,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>461</v>
       </c>
@@ -4450,7 +4455,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>463</v>
       </c>
@@ -4458,7 +4463,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>465</v>
       </c>
@@ -4466,7 +4471,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>467</v>
       </c>
@@ -4474,7 +4479,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>469</v>
       </c>
@@ -4482,7 +4487,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>471</v>
       </c>
@@ -4490,7 +4495,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>473</v>
       </c>
@@ -4498,15 +4503,18 @@
         <v>474</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>475</v>
       </c>
       <c r="B251" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D251" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>477</v>
       </c>
@@ -4514,7 +4522,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>479</v>
       </c>
@@ -4522,7 +4530,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>481</v>
       </c>
@@ -4530,7 +4538,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>483</v>
       </c>
@@ -4538,7 +4546,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>485</v>
       </c>

</xml_diff>